<commit_message>
Further testing to see if reboot works while sharing content
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -439,7 +439,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col width="14.33203125" customWidth="1" min="1" max="4"/>
   </cols>
@@ -502,8 +502,10 @@
           <t>172.16.131.99</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>200</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Idle</t>
+        </is>
       </c>
     </row>
     <row r="4" ht="18" customHeight="1">

</xml_diff>

<commit_message>
Adjusted timer for production environment
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -52,15 +52,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +433,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -466,70 +460,52 @@
           <t>IP Address</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18" customHeight="1">
+    <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>993</t>
+          <t>1025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>633_5thFl_TechLabCodecPlus</t>
+          <t>633 501D</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>172.16.131.191</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="n">
+          <t>172.17.85.63</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="3" ht="18" customHeight="1">
+    <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>994</t>
+          <t>bunk</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>633ThirdAve_5Fl_TechLabRoomkitMini</t>
+          <t>bunk</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>172.16.131.99</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" ht="18" customHeight="1">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>996</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>633_5thFl_TechLabCodecPro</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>172.16.131.163</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>200</v>
+          <t>bunk</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>bunk</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>